<commit_message>
Extended output to include usage of facilities.
There is still possible further additions to output, as capex is made more complicated.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -767,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,7 +1277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Min and Max Values for CO2 Plant Size
These can be set in the input spreadsheet on the restrictions table.
Default setting is currently 30MW -> 400MW, but this is liable to
change.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -355,7 +355,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="833">
   <si>
     <t>Name</t>
   </si>
@@ -2848,6 +2848,12 @@
   </si>
   <si>
     <t>Lifetime</t>
+  </si>
+  <si>
+    <t>MaxCO2PlantSize</t>
+  </si>
+  <si>
+    <t>MinCO2PlantSize</t>
   </si>
 </sst>
 </file>
@@ -13220,15 +13226,22 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -13238,8 +13251,14 @@
       <c r="C1" t="s">
         <v>830</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>832</v>
+      </c>
+      <c r="E1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>96-(121*0.0732)</f>
         <v>87.142799999999994</v>
@@ -13249,6 +13268,12 @@
       </c>
       <c r="C2">
         <v>20</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+      <c r="E2">
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Getting closer to SOS
in input, have changed demand so as to use multiple co2 locations
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -3331,8 +3331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3375,7 +3375,7 @@
         <v>27</v>
       </c>
       <c r="E2">
-        <v>858</v>
+        <v>850008</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3457,7 +3457,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13874,7 +13874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Now includes the K of the objective function, and thus, isopen for locations works.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -3214,7 +3214,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3271,7 +3271,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>9999999</v>
+        <v>99999999</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3317,7 +3317,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>9999999</v>
+        <v>99999999</v>
       </c>
     </row>
   </sheetData>
@@ -3331,7 +3331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -3456,8 +3456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3551,7 +3551,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>999999</v>
+        <v>99999999</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -3589,7 +3589,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2">
-        <v>999999</v>
+        <v>99999999</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
@@ -3621,7 +3621,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="2">
-        <v>999999</v>
+        <v>99999999</v>
       </c>
       <c r="G4" t="s">
         <v>19</v>
@@ -3653,7 +3653,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>999999</v>
+        <v>99999999</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
@@ -3685,7 +3685,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="2">
-        <v>999999</v>
+        <v>99999999</v>
       </c>
       <c r="G6" t="s">
         <v>7</v>
@@ -3718,7 +3718,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="2">
-        <v>999999</v>
+        <v>99999999</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -3751,7 +3751,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="2">
-        <v>999999</v>
+        <v>99999999</v>
       </c>
       <c r="G8" t="s">
         <v>29</v>
@@ -3784,7 +3784,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="2">
-        <v>999999</v>
+        <v>99999999</v>
       </c>
       <c r="G9" t="s">
         <v>29</v>
@@ -3817,7 +3817,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="2">
-        <v>999999</v>
+        <v>99999999</v>
       </c>
       <c r="G10" t="s">
         <v>29</v>
@@ -3850,7 +3850,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="2">
-        <v>999999</v>
+        <v>99999999</v>
       </c>
       <c r="G11" t="s">
         <v>29</v>
@@ -3883,7 +3883,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="2">
-        <v>999999</v>
+        <v>99999999</v>
       </c>
       <c r="G12" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Added calculation of the costpKg matrix and implementation into the objective function.
Needs to be checked
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -3311,7 +3311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -3554,8 +3554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3801,7 +3801,7 @@
         <v>99999999</v>
       </c>
       <c r="G6" s="2">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H6" t="s">
         <v>7</v>
@@ -4454,8 +4454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S167"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D167" sqref="D167"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4764,7 +4764,7 @@
         <v>141</v>
       </c>
       <c r="S5">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -4822,7 +4822,7 @@
         <v>114</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
with updated calculations from Max.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -3311,8 +3311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3357,7 +3357,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.01</v>
+        <v>1000</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -3380,7 +3380,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0.02</v>
+        <v>2000</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -3430,7 +3430,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3554,8 +3554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3766,7 +3766,7 @@
         <v>99999999</v>
       </c>
       <c r="G5" s="2">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H5" t="s">
         <v>7</v>
@@ -3801,7 +3801,7 @@
         <v>99999999</v>
       </c>
       <c r="G6" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H6" t="s">
         <v>7</v>
@@ -4455,7 +4455,7 @@
   <dimension ref="A1:S167"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4593,7 +4593,7 @@
         <v>199</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -4651,7 +4651,7 @@
         <v>327</v>
       </c>
       <c r="S3">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -4709,7 +4709,7 @@
         <v>152</v>
       </c>
       <c r="S4">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -4764,7 +4764,7 @@
         <v>141</v>
       </c>
       <c r="S5">
-        <v>12</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -4822,7 +4822,7 @@
         <v>114</v>
       </c>
       <c r="S6">
-        <v>11</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -4880,7 +4880,7 @@
         <v>188</v>
       </c>
       <c r="S7">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -4935,7 +4935,7 @@
         <v>134</v>
       </c>
       <c r="S8">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -4993,7 +4993,7 @@
         <v>300</v>
       </c>
       <c r="S9">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -5048,7 +5048,7 @@
         <v>109</v>
       </c>
       <c r="S10">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -5103,7 +5103,7 @@
         <v>134</v>
       </c>
       <c r="S11">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -5158,7 +5158,7 @@
         <v>109</v>
       </c>
       <c r="S12">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -5213,7 +5213,7 @@
         <v>109</v>
       </c>
       <c r="S13">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -5271,7 +5271,7 @@
         <v>275</v>
       </c>
       <c r="S14">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -5326,7 +5326,7 @@
         <v>141</v>
       </c>
       <c r="S15">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -5381,7 +5381,7 @@
         <v>141</v>
       </c>
       <c r="S16">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -5439,7 +5439,7 @@
         <v>199</v>
       </c>
       <c r="S17">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -5494,7 +5494,7 @@
         <v>109</v>
       </c>
       <c r="S18">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -5552,7 +5552,7 @@
         <v>275</v>
       </c>
       <c r="S19">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -5610,7 +5610,7 @@
         <v>152</v>
       </c>
       <c r="S20">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
@@ -5668,7 +5668,7 @@
         <v>300</v>
       </c>
       <c r="S21">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -5723,7 +5723,7 @@
         <v>109</v>
       </c>
       <c r="S22">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -5778,7 +5778,7 @@
         <v>109</v>
       </c>
       <c r="S23">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -5833,7 +5833,7 @@
         <v>109</v>
       </c>
       <c r="S24">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -5888,7 +5888,7 @@
         <v>254</v>
       </c>
       <c r="S25">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -5946,7 +5946,7 @@
         <v>376</v>
       </c>
       <c r="S26">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -6001,7 +6001,7 @@
         <v>121</v>
       </c>
       <c r="S27">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -6056,7 +6056,7 @@
         <v>151</v>
       </c>
       <c r="S28">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -6114,7 +6114,7 @@
         <v>202</v>
       </c>
       <c r="S29">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -6169,7 +6169,7 @@
         <v>109</v>
       </c>
       <c r="S30">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -6224,7 +6224,7 @@
         <v>134</v>
       </c>
       <c r="S31">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -6279,7 +6279,7 @@
         <v>254</v>
       </c>
       <c r="S32">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
@@ -6334,7 +6334,7 @@
         <v>450</v>
       </c>
       <c r="S33">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
@@ -6392,7 +6392,7 @@
         <v>188</v>
       </c>
       <c r="S34">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
@@ -6450,7 +6450,7 @@
         <v>236</v>
       </c>
       <c r="S35">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -6505,7 +6505,7 @@
         <v>141</v>
       </c>
       <c r="S36">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
@@ -6560,7 +6560,7 @@
         <v>109</v>
       </c>
       <c r="S37">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
@@ -6615,7 +6615,7 @@
         <v>121</v>
       </c>
       <c r="S38">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
@@ -6673,7 +6673,7 @@
         <v>202</v>
       </c>
       <c r="S39">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
@@ -6728,7 +6728,7 @@
         <v>254</v>
       </c>
       <c r="S40">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
@@ -6786,7 +6786,7 @@
         <v>188</v>
       </c>
       <c r="S41">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
@@ -6841,7 +6841,7 @@
         <v>109</v>
       </c>
       <c r="S42">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
@@ -6896,7 +6896,7 @@
         <v>254</v>
       </c>
       <c r="S43">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
@@ -6951,7 +6951,7 @@
         <v>134</v>
       </c>
       <c r="S44">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
@@ -7009,7 +7009,7 @@
         <v>188</v>
       </c>
       <c r="S45">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
@@ -7064,7 +7064,7 @@
         <v>134</v>
       </c>
       <c r="S46">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
@@ -7119,7 +7119,7 @@
         <v>109</v>
       </c>
       <c r="S47">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
@@ -7174,7 +7174,7 @@
         <v>109</v>
       </c>
       <c r="S48">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
@@ -7232,7 +7232,7 @@
         <v>236</v>
       </c>
       <c r="S49">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
@@ -7287,7 +7287,7 @@
         <v>524</v>
       </c>
       <c r="S50">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
@@ -7345,7 +7345,7 @@
         <v>202</v>
       </c>
       <c r="S51">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
@@ -7400,7 +7400,7 @@
         <v>208</v>
       </c>
       <c r="S52">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
@@ -7455,7 +7455,7 @@
         <v>450</v>
       </c>
       <c r="S53">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
@@ -7510,7 +7510,7 @@
         <v>208</v>
       </c>
       <c r="S54">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
@@ -7568,7 +7568,7 @@
         <v>518</v>
       </c>
       <c r="S55">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
@@ -7626,7 +7626,7 @@
         <v>552</v>
       </c>
       <c r="S56">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
@@ -7681,7 +7681,7 @@
         <v>121</v>
       </c>
       <c r="S57">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
@@ -7736,7 +7736,7 @@
         <v>109</v>
       </c>
       <c r="S58">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
@@ -7791,7 +7791,7 @@
         <v>109</v>
       </c>
       <c r="S59">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
@@ -7846,7 +7846,7 @@
         <v>109</v>
       </c>
       <c r="S60">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
@@ -7904,7 +7904,7 @@
         <v>188</v>
       </c>
       <c r="S61">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
@@ -7959,7 +7959,7 @@
         <v>109</v>
       </c>
       <c r="S62">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
@@ -8017,7 +8017,7 @@
         <v>376</v>
       </c>
       <c r="S63">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
@@ -8072,7 +8072,7 @@
         <v>109</v>
       </c>
       <c r="S64">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
@@ -8130,7 +8130,7 @@
         <v>275</v>
       </c>
       <c r="S65">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
@@ -8185,7 +8185,7 @@
         <v>109</v>
       </c>
       <c r="S66">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
@@ -8243,7 +8243,7 @@
         <v>114</v>
       </c>
       <c r="S67">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
@@ -8298,7 +8298,7 @@
         <v>141</v>
       </c>
       <c r="S68">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
@@ -8353,7 +8353,7 @@
         <v>141</v>
       </c>
       <c r="S69">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
@@ -8408,7 +8408,7 @@
         <v>208</v>
       </c>
       <c r="S70">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
@@ -8463,7 +8463,7 @@
         <v>109</v>
       </c>
       <c r="S71">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
@@ -8518,7 +8518,7 @@
         <v>100</v>
       </c>
       <c r="S72">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
@@ -8573,7 +8573,7 @@
         <v>609</v>
       </c>
       <c r="S73">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.25">
@@ -8631,7 +8631,7 @@
         <v>275</v>
       </c>
       <c r="S74">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
@@ -8686,7 +8686,7 @@
         <v>254</v>
       </c>
       <c r="S75">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
@@ -8741,7 +8741,7 @@
         <v>254</v>
       </c>
       <c r="S76">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.25">
@@ -8796,7 +8796,7 @@
         <v>254</v>
       </c>
       <c r="S77">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.25">
@@ -8851,7 +8851,7 @@
         <v>609</v>
       </c>
       <c r="S78">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.25">
@@ -8906,7 +8906,7 @@
         <v>254</v>
       </c>
       <c r="S79">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.25">
@@ -8961,7 +8961,7 @@
         <v>254</v>
       </c>
       <c r="S80">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.25">
@@ -9016,7 +9016,7 @@
         <v>254</v>
       </c>
       <c r="S81">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.25">
@@ -9074,7 +9074,7 @@
         <v>635</v>
       </c>
       <c r="S82">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
@@ -9129,7 +9129,7 @@
         <v>254</v>
       </c>
       <c r="S83">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.25">
@@ -9184,7 +9184,7 @@
         <v>100</v>
       </c>
       <c r="S84">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.25">
@@ -9239,7 +9239,7 @@
         <v>109</v>
       </c>
       <c r="S85">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.25">
@@ -9294,7 +9294,7 @@
         <v>151</v>
       </c>
       <c r="S86">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.25">
@@ -9349,7 +9349,7 @@
         <v>121</v>
       </c>
       <c r="S87">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.25">
@@ -9407,7 +9407,7 @@
         <v>300</v>
       </c>
       <c r="S88">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.25">
@@ -9462,7 +9462,7 @@
         <v>109</v>
       </c>
       <c r="S89">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.25">
@@ -9517,7 +9517,7 @@
         <v>109</v>
       </c>
       <c r="S90">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.25">
@@ -9575,7 +9575,7 @@
         <v>275</v>
       </c>
       <c r="S91">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.25">
@@ -9633,7 +9633,7 @@
         <v>536</v>
       </c>
       <c r="S92">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.25">
@@ -9688,7 +9688,7 @@
         <v>121</v>
       </c>
       <c r="S93">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.25">
@@ -9746,7 +9746,7 @@
         <v>236</v>
       </c>
       <c r="S94">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.25">
@@ -9801,7 +9801,7 @@
         <v>109</v>
       </c>
       <c r="S95">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.25">
@@ -9859,7 +9859,7 @@
         <v>552</v>
       </c>
       <c r="S96">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.25">
@@ -9917,7 +9917,7 @@
         <v>275</v>
       </c>
       <c r="S97">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.25">
@@ -9972,7 +9972,7 @@
         <v>121</v>
       </c>
       <c r="S98">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.25">
@@ -10027,7 +10027,7 @@
         <v>430</v>
       </c>
       <c r="S99">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.25">
@@ -10085,7 +10085,7 @@
         <v>188</v>
       </c>
       <c r="S100">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.25">
@@ -10140,7 +10140,7 @@
         <v>109</v>
       </c>
       <c r="S101">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.25">
@@ -10198,7 +10198,7 @@
         <v>236</v>
       </c>
       <c r="S102">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.25">
@@ -10253,7 +10253,7 @@
         <v>121</v>
       </c>
       <c r="S103">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.25">
@@ -10311,7 +10311,7 @@
         <v>127</v>
       </c>
       <c r="S104">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.25">
@@ -10366,7 +10366,7 @@
         <v>134</v>
       </c>
       <c r="S105">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.25">
@@ -10421,7 +10421,7 @@
         <v>141</v>
       </c>
       <c r="S106">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.25">
@@ -10476,7 +10476,7 @@
         <v>141</v>
       </c>
       <c r="S107">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.25">
@@ -10534,7 +10534,7 @@
         <v>152</v>
       </c>
       <c r="S108">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.25">
@@ -10589,7 +10589,7 @@
         <v>109</v>
       </c>
       <c r="S109">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="110" spans="1:19" x14ac:dyDescent="0.25">
@@ -10647,7 +10647,7 @@
         <v>152</v>
       </c>
       <c r="S110">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.25">
@@ -10705,7 +10705,7 @@
         <v>114</v>
       </c>
       <c r="S111">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.25">
@@ -10760,7 +10760,7 @@
         <v>169</v>
       </c>
       <c r="S112">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.25">
@@ -10818,7 +10818,7 @@
         <v>175</v>
       </c>
       <c r="S113">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.25">
@@ -10873,7 +10873,7 @@
         <v>182</v>
       </c>
       <c r="S114">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.25">
@@ -10931,7 +10931,7 @@
         <v>188</v>
       </c>
       <c r="S115">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="116" spans="1:19" x14ac:dyDescent="0.25">
@@ -10986,7 +10986,7 @@
         <v>109</v>
       </c>
       <c r="S116">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="117" spans="1:19" x14ac:dyDescent="0.25">
@@ -11044,7 +11044,7 @@
         <v>199</v>
       </c>
       <c r="S117">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="118" spans="1:19" x14ac:dyDescent="0.25">
@@ -11102,7 +11102,7 @@
         <v>202</v>
       </c>
       <c r="S118">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="119" spans="1:19" x14ac:dyDescent="0.25">
@@ -11157,7 +11157,7 @@
         <v>208</v>
       </c>
       <c r="S119">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.25">
@@ -11212,7 +11212,7 @@
         <v>215</v>
       </c>
       <c r="S120">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.25">
@@ -11267,7 +11267,7 @@
         <v>151</v>
       </c>
       <c r="S121">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.25">
@@ -11322,7 +11322,7 @@
         <v>706</v>
       </c>
       <c r="S122">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="123" spans="1:19" x14ac:dyDescent="0.25">
@@ -11377,7 +11377,7 @@
         <v>706</v>
       </c>
       <c r="S123">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="124" spans="1:19" x14ac:dyDescent="0.25">
@@ -11432,7 +11432,7 @@
         <v>706</v>
       </c>
       <c r="S124">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.25">
@@ -11487,7 +11487,7 @@
         <v>109</v>
       </c>
       <c r="S125">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="126" spans="1:19" x14ac:dyDescent="0.25">
@@ -11542,7 +11542,7 @@
         <v>100</v>
       </c>
       <c r="S126">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="127" spans="1:19" x14ac:dyDescent="0.25">
@@ -11597,7 +11597,7 @@
         <v>141</v>
       </c>
       <c r="S127">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="128" spans="1:19" x14ac:dyDescent="0.25">
@@ -11652,7 +11652,7 @@
         <v>100</v>
       </c>
       <c r="S128">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="129" spans="1:19" x14ac:dyDescent="0.25">
@@ -11707,7 +11707,7 @@
         <v>109</v>
       </c>
       <c r="S129">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="130" spans="1:19" x14ac:dyDescent="0.25">
@@ -11762,7 +11762,7 @@
         <v>100</v>
       </c>
       <c r="S130">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="131" spans="1:19" x14ac:dyDescent="0.25">
@@ -11817,7 +11817,7 @@
         <v>141</v>
       </c>
       <c r="S131">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="132" spans="1:19" x14ac:dyDescent="0.25">
@@ -11875,7 +11875,7 @@
         <v>300</v>
       </c>
       <c r="S132">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="133" spans="1:19" x14ac:dyDescent="0.25">
@@ -11930,7 +11930,7 @@
         <v>121</v>
       </c>
       <c r="S133">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="134" spans="1:19" x14ac:dyDescent="0.25">
@@ -11988,7 +11988,7 @@
         <v>635</v>
       </c>
       <c r="S134">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="135" spans="1:19" x14ac:dyDescent="0.25">
@@ -12043,7 +12043,7 @@
         <v>109</v>
       </c>
       <c r="S135">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="136" spans="1:19" x14ac:dyDescent="0.25">
@@ -12098,7 +12098,7 @@
         <v>134</v>
       </c>
       <c r="S136">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="137" spans="1:19" x14ac:dyDescent="0.25">
@@ -12153,7 +12153,7 @@
         <v>208</v>
       </c>
       <c r="S137">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.25">
@@ -12208,7 +12208,7 @@
         <v>109</v>
       </c>
       <c r="S138">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="139" spans="1:19" x14ac:dyDescent="0.25">
@@ -12263,7 +12263,7 @@
         <v>134</v>
       </c>
       <c r="S139">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="140" spans="1:19" x14ac:dyDescent="0.25">
@@ -12321,7 +12321,7 @@
         <v>202</v>
       </c>
       <c r="S140">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="141" spans="1:19" x14ac:dyDescent="0.25">
@@ -12376,7 +12376,7 @@
         <v>141</v>
       </c>
       <c r="S141">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="142" spans="1:19" x14ac:dyDescent="0.25">
@@ -12431,7 +12431,7 @@
         <v>134</v>
       </c>
       <c r="S142">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="143" spans="1:19" x14ac:dyDescent="0.25">
@@ -12486,7 +12486,7 @@
         <v>254</v>
       </c>
       <c r="S143">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="144" spans="1:19" x14ac:dyDescent="0.25">
@@ -12541,7 +12541,7 @@
         <v>134</v>
       </c>
       <c r="S144">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="145" spans="1:19" x14ac:dyDescent="0.25">
@@ -12599,7 +12599,7 @@
         <v>188</v>
       </c>
       <c r="S145">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="146" spans="1:19" x14ac:dyDescent="0.25">
@@ -12654,7 +12654,7 @@
         <v>109</v>
       </c>
       <c r="S146">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="147" spans="1:19" x14ac:dyDescent="0.25">
@@ -12709,7 +12709,7 @@
         <v>450</v>
       </c>
       <c r="S147">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="148" spans="1:19" x14ac:dyDescent="0.25">
@@ -12764,7 +12764,7 @@
         <v>450</v>
       </c>
       <c r="S148">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="149" spans="1:19" x14ac:dyDescent="0.25">
@@ -12819,7 +12819,7 @@
         <v>450</v>
       </c>
       <c r="S149">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="150" spans="1:19" x14ac:dyDescent="0.25">
@@ -12877,7 +12877,7 @@
         <v>236</v>
       </c>
       <c r="S150">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="151" spans="1:19" x14ac:dyDescent="0.25">
@@ -12935,7 +12935,7 @@
         <v>236</v>
       </c>
       <c r="S151">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="152" spans="1:19" x14ac:dyDescent="0.25">
@@ -12993,7 +12993,7 @@
         <v>236</v>
       </c>
       <c r="S152">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="153" spans="1:19" x14ac:dyDescent="0.25">
@@ -13048,7 +13048,7 @@
         <v>121</v>
       </c>
       <c r="S153">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="154" spans="1:19" x14ac:dyDescent="0.25">
@@ -13106,7 +13106,7 @@
         <v>175</v>
       </c>
       <c r="S154">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="155" spans="1:19" x14ac:dyDescent="0.25">
@@ -13161,7 +13161,7 @@
         <v>134</v>
       </c>
       <c r="S155">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="156" spans="1:19" x14ac:dyDescent="0.25">
@@ -13216,7 +13216,7 @@
         <v>121</v>
       </c>
       <c r="S156">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="157" spans="1:19" x14ac:dyDescent="0.25">
@@ -13271,7 +13271,7 @@
         <v>134</v>
       </c>
       <c r="S157">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="158" spans="1:19" x14ac:dyDescent="0.25">
@@ -13329,7 +13329,7 @@
         <v>188</v>
       </c>
       <c r="S158">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="159" spans="1:19" x14ac:dyDescent="0.25">
@@ -13384,7 +13384,7 @@
         <v>134</v>
       </c>
       <c r="S159">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="160" spans="1:19" x14ac:dyDescent="0.25">
@@ -13439,7 +13439,7 @@
         <v>254</v>
       </c>
       <c r="S160">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="161" spans="1:19" x14ac:dyDescent="0.25">
@@ -13494,7 +13494,7 @@
         <v>109</v>
       </c>
       <c r="S161">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="162" spans="1:19" x14ac:dyDescent="0.25">
@@ -13549,7 +13549,7 @@
         <v>793</v>
       </c>
       <c r="S162">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="163" spans="1:19" x14ac:dyDescent="0.25">
@@ -13607,7 +13607,7 @@
         <v>101</v>
       </c>
       <c r="S163">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="164" spans="1:19" x14ac:dyDescent="0.25">
@@ -13662,7 +13662,7 @@
         <v>109</v>
       </c>
       <c r="S164">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="165" spans="1:19" x14ac:dyDescent="0.25">
@@ -13720,7 +13720,7 @@
         <v>114</v>
       </c>
       <c r="S165">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="166" spans="1:19" x14ac:dyDescent="0.25">
@@ -13775,7 +13775,7 @@
         <v>121</v>
       </c>
       <c r="S166">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="167" spans="1:19" x14ac:dyDescent="0.25">
@@ -13830,7 +13830,7 @@
         <v>121</v>
       </c>
       <c r="S167">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made a few minor cosmetic changes
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -13,7 +13,8 @@
     <sheet name="Connectors" sheetId="4" r:id="rId4"/>
     <sheet name="Hubs" sheetId="5" r:id="rId5"/>
     <sheet name="CO2Locations" sheetId="7" r:id="rId6"/>
-    <sheet name="Restrictions" sheetId="6" r:id="rId7"/>
+    <sheet name="FuelCharacteristics" sheetId="8" r:id="rId7"/>
+    <sheet name="Restrictions" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -355,7 +356,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1758" uniqueCount="836">
   <si>
     <t>Name</t>
   </si>
@@ -2860,6 +2861,9 @@
   </si>
   <si>
     <t>CO2 Cost pkg</t>
+  </si>
+  <si>
+    <t>EnergyDensity</t>
   </si>
 </sst>
 </file>
@@ -3312,7 +3316,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3555,7 +3559,7 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4455,7 +4459,7 @@
   <dimension ref="A1:S167"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4477,6 +4481,7 @@
     <col min="16" max="16" width="20.42578125" customWidth="1"/>
     <col min="17" max="17" width="21.5703125" customWidth="1"/>
     <col min="18" max="18" width="24.85546875" customWidth="1"/>
+    <col min="19" max="19" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -13842,11 +13847,34 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Initial visualization efforts. need to check for corectness and prevent overwriting
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -283,7 +283,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1836" uniqueCount="856">
   <si>
     <t>Name</t>
   </si>
@@ -2845,6 +2845,12 @@
   </si>
   <si>
     <t>4-ker</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -3304,10 +3310,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3321,7 +3327,7 @@
     <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3343,8 +3349,14 @@
       <c r="G1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>854</v>
+      </c>
+      <c r="I1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -3366,8 +3378,14 @@
       <c r="G2" s="5">
         <v>999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
@@ -3389,8 +3407,14 @@
       <c r="G3" s="5">
         <v>400</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="12">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -3412,8 +3436,14 @@
       <c r="G4" s="5">
         <v>999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="12">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>829</v>
       </c>
@@ -3434,6 +3464,12 @@
       </c>
       <c r="G5" s="5">
         <v>999999</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3445,10 +3481,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3460,7 +3496,7 @@
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3476,8 +3512,14 @@
       <c r="E1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>854</v>
+      </c>
+      <c r="G1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
@@ -3493,8 +3535,14 @@
       <c r="E2" s="6">
         <v>858</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="12">
+        <v>320</v>
+      </c>
+      <c r="G2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>54</v>
       </c>
@@ -3510,8 +3558,14 @@
       <c r="E3" s="6">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="12">
+        <v>320</v>
+      </c>
+      <c r="G3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>55</v>
       </c>
@@ -3527,8 +3581,14 @@
       <c r="E4" s="6">
         <v>24.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="12">
+        <v>320</v>
+      </c>
+      <c r="G4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>56</v>
       </c>
@@ -3544,8 +3604,14 @@
       <c r="E5" s="6">
         <v>130.30000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="12">
+        <v>320</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>57</v>
       </c>
@@ -3561,8 +3627,14 @@
       <c r="E6" s="6">
         <v>414.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="12">
+        <v>320</v>
+      </c>
+      <c r="G6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>831</v>
       </c>
@@ -3577,6 +3649,12 @@
       </c>
       <c r="E7" s="6">
         <v>120</v>
+      </c>
+      <c r="F7" s="12">
+        <v>320</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3587,10 +3665,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H2" sqref="H2:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3601,23 +3679,24 @@
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" customWidth="1"/>
     <col min="6" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="9.42578125" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.85546875" style="12" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="15" width="9.42578125" customWidth="1"/>
+    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3639,38 +3718,44 @@
       <c r="G1" t="s">
         <v>827</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="12" t="s">
+        <v>854</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>855</v>
+      </c>
+      <c r="J1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>2</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>3</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -3692,34 +3777,40 @@
       <c r="G2" s="8">
         <v>0</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="8">
+        <v>80</v>
+      </c>
+      <c r="I2" s="8">
+        <v>300</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="7">
+      <c r="K2" s="7">
         <v>1</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="10">
+      <c r="O2" s="10">
         <v>0.27956989247311831</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="P2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="10">
+      <c r="Q2" s="10">
         <v>0.58064516129032262</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>831</v>
       </c>
-      <c r="Q2" s="10">
+      <c r="S2" s="10">
         <v>0.13978494623655915</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>832</v>
       </c>
@@ -3741,30 +3832,36 @@
       <c r="G3" s="8">
         <v>0</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="8">
+        <v>80</v>
+      </c>
+      <c r="I3" s="8">
+        <v>250</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="7">
+      <c r="K3" s="7">
         <v>1</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="10">
+      <c r="O3" s="10">
         <v>0.32520325203252037</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="10">
+      <c r="Q3" s="10">
         <v>0.67479674796747968</v>
       </c>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>31</v>
       </c>
@@ -3786,26 +3883,32 @@
       <c r="G4" s="8">
         <v>0</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="8">
+        <v>80</v>
+      </c>
+      <c r="I4" s="8">
+        <v>150</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="7">
+      <c r="K4" s="7">
         <v>1</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="7">
+      <c r="O4" s="7">
         <v>1</v>
       </c>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>30</v>
       </c>
@@ -3827,26 +3930,32 @@
       <c r="G5" s="8">
         <v>0</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="8">
+        <v>80</v>
+      </c>
+      <c r="I5" s="8">
+        <v>200</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="7">
+      <c r="K5" s="7">
         <v>1</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="7">
+      <c r="O5" s="7">
         <v>1</v>
       </c>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
@@ -3868,30 +3977,36 @@
       <c r="G6" s="8">
         <v>0.1</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="8">
+        <v>80</v>
+      </c>
+      <c r="I6" s="8">
+        <v>100</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="10">
+      <c r="K6" s="10">
         <v>0.92636284614429409</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="L6" s="7" t="s">
         <v>830</v>
       </c>
-      <c r="K6" s="10">
+      <c r="M6" s="10">
         <v>7.3637153855705906E-2</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="N6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="7">
+      <c r="O6" s="7">
         <v>1</v>
       </c>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>833</v>
       </c>
@@ -3913,34 +4028,40 @@
       <c r="G7" s="8">
         <v>0.1</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="8">
+        <v>80</v>
+      </c>
+      <c r="I7" s="8">
+        <v>50</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="10">
+      <c r="K7" s="10">
         <v>0.90716180371352784</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="L7" s="7" t="s">
         <v>830</v>
       </c>
-      <c r="K7" s="10">
+      <c r="M7" s="10">
         <v>9.2838196286472163E-2</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="N7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="10">
+      <c r="O7" s="10">
         <v>0.30902777777777785</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="P7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O7" s="10">
+      <c r="Q7" s="10">
         <v>0.6909722222222221</v>
       </c>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>834</v>
       </c>
@@ -3962,38 +4083,44 @@
       <c r="G8" s="8">
         <v>0.1</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="8">
+        <v>80</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="10">
+      <c r="K8" s="10">
         <v>0.90716180371352784</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="L8" s="7" t="s">
         <v>830</v>
       </c>
-      <c r="K8" s="10">
+      <c r="M8" s="10">
         <v>9.2838196286472163E-2</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="N8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="10">
+      <c r="O8" s="10">
         <v>0.245</v>
       </c>
-      <c r="N8" s="7" t="s">
+      <c r="P8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O8" s="10">
+      <c r="Q8" s="10">
         <v>3.0000000000000002E-2</v>
       </c>
-      <c r="P8" s="7" t="s">
+      <c r="R8" s="7" t="s">
         <v>831</v>
       </c>
-      <c r="Q8" s="10">
+      <c r="S8" s="10">
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>50</v>
       </c>
@@ -4015,26 +4142,32 @@
       <c r="G9" s="8">
         <v>0</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="8">
+        <v>240</v>
+      </c>
+      <c r="I9" s="8">
+        <v>300</v>
+      </c>
+      <c r="J9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="7">
+      <c r="K9" s="7">
         <v>1</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7" t="s">
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="7">
+      <c r="O9" s="7">
         <v>1</v>
       </c>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>51</v>
       </c>
@@ -4056,26 +4189,32 @@
       <c r="G10" s="8">
         <v>0</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="8">
+        <v>240</v>
+      </c>
+      <c r="I10" s="8">
+        <v>250</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="7">
+      <c r="K10" s="7">
         <v>1</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7" t="s">
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="M10" s="7">
+      <c r="O10" s="7">
         <v>1</v>
       </c>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>44</v>
       </c>
@@ -4097,26 +4236,32 @@
       <c r="G11" s="8">
         <v>0</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="8">
+        <v>240</v>
+      </c>
+      <c r="I11" s="8">
+        <v>200</v>
+      </c>
+      <c r="J11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="7">
+      <c r="K11" s="7">
         <v>1</v>
       </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7" t="s">
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="M11" s="7">
+      <c r="O11" s="7">
         <v>1</v>
       </c>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>45</v>
       </c>
@@ -4138,22 +4283,28 @@
       <c r="G12" s="8">
         <v>0</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="8">
+        <v>240</v>
+      </c>
+      <c r="I12" s="8">
+        <v>150</v>
+      </c>
+      <c r="J12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="7">
+      <c r="K12" s="7">
         <v>1</v>
       </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7" t="s">
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="M12" s="7">
+      <c r="O12" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>58</v>
       </c>
@@ -4175,22 +4326,28 @@
       <c r="G13" s="8">
         <v>0</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="8">
+        <v>240</v>
+      </c>
+      <c r="I13" s="8">
+        <v>100</v>
+      </c>
+      <c r="J13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="7">
+      <c r="K13" s="7">
         <v>1</v>
       </c>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7" t="s">
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="M13" s="7">
+      <c r="O13" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>59</v>
       </c>
@@ -4212,18 +4369,24 @@
       <c r="G14" s="8">
         <v>0</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="8">
+        <v>240</v>
+      </c>
+      <c r="I14" s="8">
+        <v>50</v>
+      </c>
+      <c r="J14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="7">
+      <c r="K14" s="7">
         <v>1</v>
       </c>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7" t="s">
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="M14" s="7">
+      <c r="O14" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4238,7 +4401,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4773,15 +4936,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4794,8 +4957,14 @@
       <c r="D1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>854</v>
+      </c>
+      <c r="F1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>35</v>
       </c>
@@ -4808,8 +4977,14 @@
       <c r="D2" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>160</v>
+      </c>
+      <c r="F2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>36</v>
       </c>
@@ -4822,8 +4997,14 @@
       <c r="D3" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="12">
+        <v>160</v>
+      </c>
+      <c r="F3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>845</v>
       </c>
@@ -4835,6 +5016,12 @@
       </c>
       <c r="D4" s="12">
         <v>0</v>
+      </c>
+      <c r="E4" s="12">
+        <v>160</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Experiment some with specific energies
Nothing permanent, mainly just doing this so I can merge with the
graphical version. Regardless, some work has been done on developing the
specific energy read ins.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="Hubs" sheetId="5" r:id="rId5"/>
     <sheet name="CO2Locations" sheetId="7" r:id="rId6"/>
     <sheet name="Restrictions" sheetId="6" r:id="rId7"/>
+    <sheet name="EnergyTypes" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -282,8 +283,43 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In MJ/kg
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1836" uniqueCount="856">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1841" uniqueCount="857">
   <si>
     <t>Name</t>
   </si>
@@ -2851,6 +2887,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>EnergyDensity</t>
   </si>
 </sst>
 </file>
@@ -2860,7 +2899,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2896,6 +2935,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -3312,7 +3364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -3668,7 +3720,7 @@
   <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H8"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14475,4 +14527,56 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>46.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>831</v>
+      </c>
+      <c r="B4">
+        <v>42.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added indOpex reliance on specific energy
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -220,7 +220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -319,7 +319,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1841" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="858">
   <si>
     <t>Name</t>
   </si>
@@ -2890,6 +2890,9 @@
   </si>
   <si>
     <t>EnergyDensity</t>
+  </si>
+  <si>
+    <t>OutputSpecEnergy</t>
   </si>
 </sst>
 </file>
@@ -3717,10 +3720,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3730,25 +3733,28 @@
     <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="9" width="11.85546875" style="12" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="15" width="9.42578125" customWidth="1"/>
-    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="3.28515625" style="12" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" style="12" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="16" width="9.42578125" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3767,47 +3773,50 @@
       <c r="F1" t="s">
         <v>65</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="12" t="s">
+        <v>857</v>
+      </c>
+      <c r="H1" t="s">
         <v>827</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>854</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>855</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>25</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>16</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>17</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>3</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>42</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -3830,39 +3839,42 @@
         <v>0</v>
       </c>
       <c r="H2" s="8">
+        <v>0</v>
+      </c>
+      <c r="I2" s="8">
         <v>80</v>
       </c>
-      <c r="I2" s="8">
+      <c r="J2" s="8">
         <v>300</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="7">
+      <c r="L2" s="7">
         <v>1</v>
       </c>
-      <c r="L2" s="7"/>
       <c r="M2" s="7"/>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="7"/>
+      <c r="O2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="10">
+      <c r="P2" s="10">
         <v>0.27956989247311831</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="Q2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="10">
+      <c r="R2" s="10">
         <v>0.58064516129032262</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>831</v>
       </c>
-      <c r="S2" s="10">
+      <c r="T2" s="10">
         <v>0.13978494623655915</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>832</v>
       </c>
@@ -3881,39 +3893,42 @@
       <c r="F3" s="7">
         <v>999999</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="12">
         <v>0</v>
       </c>
       <c r="H3" s="8">
+        <v>0</v>
+      </c>
+      <c r="I3" s="8">
         <v>80</v>
       </c>
-      <c r="I3" s="8">
+      <c r="J3" s="8">
         <v>250</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="7">
+      <c r="L3" s="7">
         <v>1</v>
       </c>
-      <c r="L3" s="7"/>
       <c r="M3" s="7"/>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="7"/>
+      <c r="O3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="10">
+      <c r="P3" s="10">
         <v>0.32520325203252037</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="Q3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="10">
+      <c r="R3" s="10">
         <v>0.67479674796747968</v>
       </c>
-      <c r="R3" s="7"/>
       <c r="S3" s="7"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T3" s="7"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>31</v>
       </c>
@@ -3936,31 +3951,34 @@
         <v>0</v>
       </c>
       <c r="H4" s="8">
+        <v>0</v>
+      </c>
+      <c r="I4" s="8">
         <v>80</v>
       </c>
-      <c r="I4" s="8">
+      <c r="J4" s="8">
         <v>150</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="7">
+      <c r="L4" s="7">
         <v>1</v>
       </c>
-      <c r="L4" s="7"/>
       <c r="M4" s="7"/>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="7"/>
+      <c r="O4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O4" s="7">
+      <c r="P4" s="7">
         <v>1</v>
       </c>
-      <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T4" s="7"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>30</v>
       </c>
@@ -3983,31 +4001,34 @@
         <v>0</v>
       </c>
       <c r="H5" s="8">
+        <v>0</v>
+      </c>
+      <c r="I5" s="8">
         <v>80</v>
       </c>
-      <c r="I5" s="8">
+      <c r="J5" s="8">
         <v>200</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="7">
+      <c r="L5" s="7">
         <v>1</v>
       </c>
-      <c r="L5" s="7"/>
       <c r="M5" s="7"/>
-      <c r="N5" s="7" t="s">
+      <c r="N5" s="7"/>
+      <c r="O5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="O5" s="7">
+      <c r="P5" s="7">
         <v>1</v>
       </c>
-      <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5" s="7"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
@@ -4027,38 +4048,41 @@
         <v>999999</v>
       </c>
       <c r="G6" s="8">
+        <v>43.1</v>
+      </c>
+      <c r="H6" s="8">
         <v>0.1</v>
       </c>
-      <c r="H6" s="8">
+      <c r="I6" s="8">
         <v>80</v>
       </c>
-      <c r="I6" s="8">
-        <v>100</v>
-      </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="8">
+        <v>100</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="10">
+      <c r="L6" s="10">
         <v>0.92636284614429409</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="M6" s="7" t="s">
         <v>830</v>
       </c>
-      <c r="M6" s="10">
+      <c r="N6" s="10">
         <v>7.3637153855705906E-2</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="O6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="7">
+      <c r="P6" s="7">
         <v>1</v>
       </c>
-      <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T6" s="7"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>833</v>
       </c>
@@ -4078,42 +4102,45 @@
         <v>999999</v>
       </c>
       <c r="G7" s="8">
+        <v>43.1</v>
+      </c>
+      <c r="H7" s="8">
         <v>0.1</v>
       </c>
-      <c r="H7" s="8">
+      <c r="I7" s="8">
         <v>80</v>
       </c>
-      <c r="I7" s="8">
+      <c r="J7" s="8">
         <v>50</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="10">
+      <c r="L7" s="10">
         <v>0.90716180371352784</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="M7" s="7" t="s">
         <v>830</v>
       </c>
-      <c r="M7" s="10">
+      <c r="N7" s="10">
         <v>9.2838196286472163E-2</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="O7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="O7" s="10">
+      <c r="P7" s="10">
         <v>0.30902777777777785</v>
       </c>
-      <c r="P7" s="7" t="s">
+      <c r="Q7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Q7" s="10">
+      <c r="R7" s="10">
         <v>0.6909722222222221</v>
       </c>
-      <c r="R7" s="7"/>
       <c r="S7" s="7"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T7" s="7"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>834</v>
       </c>
@@ -4133,46 +4160,49 @@
         <v>999999</v>
       </c>
       <c r="G8" s="8">
+        <v>43.1</v>
+      </c>
+      <c r="H8" s="8">
         <v>0.1</v>
       </c>
-      <c r="H8" s="8">
+      <c r="I8" s="8">
         <v>80</v>
       </c>
-      <c r="I8" s="8">
+      <c r="J8" s="8">
         <v>0</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="K8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="10">
+      <c r="L8" s="10">
         <v>0.90716180371352784</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="M8" s="7" t="s">
         <v>830</v>
       </c>
-      <c r="M8" s="10">
+      <c r="N8" s="10">
         <v>9.2838196286472163E-2</v>
       </c>
-      <c r="N8" s="7" t="s">
+      <c r="O8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="O8" s="10">
+      <c r="P8" s="10">
         <v>0.245</v>
       </c>
-      <c r="P8" s="7" t="s">
+      <c r="Q8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Q8" s="10">
+      <c r="R8" s="10">
         <v>3.0000000000000002E-2</v>
       </c>
-      <c r="R8" s="7" t="s">
+      <c r="S8" s="7" t="s">
         <v>831</v>
       </c>
-      <c r="S8" s="10">
+      <c r="T8" s="10">
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>50</v>
       </c>
@@ -4195,31 +4225,34 @@
         <v>0</v>
       </c>
       <c r="H9" s="8">
+        <v>0</v>
+      </c>
+      <c r="I9" s="8">
         <v>240</v>
       </c>
-      <c r="I9" s="8">
+      <c r="J9" s="8">
         <v>300</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="K9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="7">
+      <c r="L9" s="7">
         <v>1</v>
       </c>
-      <c r="L9" s="7"/>
       <c r="M9" s="7"/>
-      <c r="N9" s="7" t="s">
+      <c r="N9" s="7"/>
+      <c r="O9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="O9" s="7">
+      <c r="P9" s="7">
         <v>1</v>
       </c>
-      <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T9" s="7"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>51</v>
       </c>
@@ -4242,31 +4275,34 @@
         <v>0</v>
       </c>
       <c r="H10" s="8">
+        <v>0</v>
+      </c>
+      <c r="I10" s="8">
         <v>240</v>
       </c>
-      <c r="I10" s="8">
+      <c r="J10" s="8">
         <v>250</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="K10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K10" s="7">
+      <c r="L10" s="7">
         <v>1</v>
       </c>
-      <c r="L10" s="7"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="7" t="s">
+      <c r="N10" s="7"/>
+      <c r="O10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="O10" s="7">
+      <c r="P10" s="7">
         <v>1</v>
       </c>
-      <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T10" s="7"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>44</v>
       </c>
@@ -4289,31 +4325,34 @@
         <v>0</v>
       </c>
       <c r="H11" s="8">
+        <v>0</v>
+      </c>
+      <c r="I11" s="8">
         <v>240</v>
       </c>
-      <c r="I11" s="8">
+      <c r="J11" s="8">
         <v>200</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="K11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K11" s="7">
+      <c r="L11" s="7">
         <v>1</v>
       </c>
-      <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="7" t="s">
+      <c r="N11" s="7"/>
+      <c r="O11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="O11" s="7">
+      <c r="P11" s="7">
         <v>1</v>
       </c>
-      <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11" s="7"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>45</v>
       </c>
@@ -4336,27 +4375,30 @@
         <v>0</v>
       </c>
       <c r="H12" s="8">
+        <v>0</v>
+      </c>
+      <c r="I12" s="8">
         <v>240</v>
       </c>
-      <c r="I12" s="8">
+      <c r="J12" s="8">
         <v>150</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="K12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K12" s="7">
+      <c r="L12" s="7">
         <v>1</v>
       </c>
-      <c r="L12" s="7"/>
       <c r="M12" s="7"/>
-      <c r="N12" s="7" t="s">
+      <c r="N12" s="7"/>
+      <c r="O12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="O12" s="7">
+      <c r="P12" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>58</v>
       </c>
@@ -4379,27 +4421,30 @@
         <v>0</v>
       </c>
       <c r="H13" s="8">
+        <v>0</v>
+      </c>
+      <c r="I13" s="8">
         <v>240</v>
       </c>
-      <c r="I13" s="8">
-        <v>100</v>
-      </c>
-      <c r="J13" s="7" t="s">
+      <c r="J13" s="8">
+        <v>100</v>
+      </c>
+      <c r="K13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K13" s="7">
+      <c r="L13" s="7">
         <v>1</v>
       </c>
-      <c r="L13" s="7"/>
       <c r="M13" s="7"/>
-      <c r="N13" s="7" t="s">
+      <c r="N13" s="7"/>
+      <c r="O13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="O13" s="7">
+      <c r="P13" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>59</v>
       </c>
@@ -4422,23 +4467,26 @@
         <v>0</v>
       </c>
       <c r="H14" s="8">
+        <v>0</v>
+      </c>
+      <c r="I14" s="8">
         <v>240</v>
       </c>
-      <c r="I14" s="8">
+      <c r="J14" s="8">
         <v>50</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="K14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="7">
+      <c r="L14" s="7">
         <v>1</v>
       </c>
-      <c r="L14" s="7"/>
       <c r="M14" s="7"/>
-      <c r="N14" s="7" t="s">
+      <c r="N14" s="7"/>
+      <c r="O14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="O14" s="7">
+      <c r="P14" s="7">
         <v>1</v>
       </c>
     </row>
@@ -14533,8 +14581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Working on adding CO2 dependent hydrogen capacity
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -3862,8 +3862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5926,8 +5926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S167"/>
   <sheetViews>
-    <sheetView topLeftCell="J130" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15317,7 +15317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Outlined multiple cost curves
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -319,7 +319,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1939" uniqueCount="887">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1961" uniqueCount="891">
   <si>
     <t>Name</t>
   </si>
@@ -2980,6 +2980,18 @@
   </si>
   <si>
     <t>1-EC_4</t>
+  </si>
+  <si>
+    <t>H2 Process</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>FT</t>
+  </si>
+  <si>
+    <t>Meth</t>
   </si>
 </sst>
 </file>
@@ -3860,10 +3872,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W22"/>
+  <dimension ref="A1:X22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3876,25 +3888,26 @@
     <col min="6" max="6" width="11.85546875" customWidth="1"/>
     <col min="7" max="7" width="21.42578125" style="11" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="5" style="11" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" style="11" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="16" width="9.42578125" customWidth="1"/>
-    <col min="17" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" style="36" customWidth="1"/>
+    <col min="10" max="10" width="5" style="11" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" style="11" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="9.42578125" customWidth="1"/>
+    <col min="18" max="18" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3919,44 +3932,47 @@
       <c r="H1" t="s">
         <v>827</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="36" t="s">
+        <v>887</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>854</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>855</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>24</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>25</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>26</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>16</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>2</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>3</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>42</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -3981,40 +3997,43 @@
       <c r="H2" s="8">
         <v>0</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="34" t="s">
+        <v>888</v>
+      </c>
+      <c r="J2" s="8">
         <v>80</v>
       </c>
-      <c r="J2" s="8">
+      <c r="K2" s="8">
         <v>250</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="7">
+      <c r="M2" s="7">
         <v>1</v>
       </c>
-      <c r="M2" s="7"/>
       <c r="N2" s="7"/>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="7"/>
+      <c r="P2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="10">
+      <c r="Q2" s="10">
         <v>0.27956989247311831</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="R2" s="10">
+      <c r="S2" s="10">
         <v>0.58064516129032262</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="T2" s="7" t="s">
         <v>831</v>
       </c>
-      <c r="T2" s="10">
+      <c r="U2" s="10">
         <v>0.13978494623655915</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>832</v>
       </c>
@@ -4039,36 +4058,39 @@
       <c r="H3" s="8">
         <v>0</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="34" t="s">
+        <v>888</v>
+      </c>
+      <c r="J3" s="8">
         <v>80</v>
       </c>
-      <c r="J3" s="8">
+      <c r="K3" s="8">
         <v>300</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="L3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="7">
+      <c r="M3" s="7">
         <v>1</v>
       </c>
-      <c r="M3" s="7"/>
       <c r="N3" s="7"/>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="7"/>
+      <c r="P3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="10">
+      <c r="Q3" s="10">
         <v>0.32520325203252037</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="R3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="R3" s="10">
+      <c r="S3" s="10">
         <v>0.67479674796747968</v>
       </c>
-      <c r="S3" s="7"/>
       <c r="T3" s="7"/>
-    </row>
-    <row r="4" spans="1:23" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U3" s="7"/>
+    </row>
+    <row r="4" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>860</v>
       </c>
@@ -4093,33 +4115,36 @@
       <c r="H4" s="14">
         <v>0</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="34" t="s">
+        <v>888</v>
+      </c>
+      <c r="J4" s="14">
         <v>80</v>
       </c>
-      <c r="J4" s="15">
+      <c r="K4" s="15">
         <v>130</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="L4" s="14" t="s">
         <v>859</v>
       </c>
-      <c r="L4" s="14">
+      <c r="M4" s="14">
         <v>1</v>
       </c>
-      <c r="M4" s="14"/>
       <c r="N4" s="14"/>
-      <c r="O4" s="14" t="s">
+      <c r="O4" s="14"/>
+      <c r="P4" s="14" t="s">
         <v>861</v>
       </c>
-      <c r="P4" s="14">
+      <c r="Q4" s="14">
         <v>1</v>
       </c>
-      <c r="Q4" s="14"/>
       <c r="R4" s="14"/>
       <c r="S4" s="14"/>
       <c r="T4" s="14"/>
-      <c r="U4" s="13"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U4" s="14"/>
+      <c r="V4" s="13"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>31</v>
       </c>
@@ -4144,32 +4169,35 @@
       <c r="H5" s="8">
         <v>0</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="34" t="s">
+        <v>888</v>
+      </c>
+      <c r="J5" s="8">
         <v>80</v>
       </c>
-      <c r="J5" s="8">
+      <c r="K5" s="8">
         <v>190</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="L5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="7">
+      <c r="M5" s="7">
         <v>1</v>
       </c>
-      <c r="M5" s="7"/>
       <c r="N5" s="7"/>
-      <c r="O5" s="7" t="s">
+      <c r="O5" s="7"/>
+      <c r="P5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="P5" s="7">
+      <c r="Q5" s="7">
         <v>1</v>
       </c>
-      <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U5" s="7"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>30</v>
       </c>
@@ -4194,32 +4222,35 @@
       <c r="H6" s="8">
         <v>0</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="34" t="s">
+        <v>888</v>
+      </c>
+      <c r="J6" s="8">
         <v>80</v>
       </c>
-      <c r="J6" s="8">
+      <c r="K6" s="8">
         <v>220</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="L6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="7">
+      <c r="M6" s="7">
         <v>1</v>
       </c>
-      <c r="M6" s="7"/>
       <c r="N6" s="7"/>
-      <c r="O6" s="7" t="s">
+      <c r="O6" s="7"/>
+      <c r="P6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="7">
+      <c r="Q6" s="7">
         <v>1</v>
       </c>
-      <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
-    </row>
-    <row r="7" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U6" s="7"/>
+    </row>
+    <row r="7" spans="1:24" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>862</v>
       </c>
@@ -4244,32 +4275,35 @@
       <c r="H7" s="18">
         <v>0</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="34" t="s">
+        <v>888</v>
+      </c>
+      <c r="J7" s="18">
         <v>80</v>
       </c>
-      <c r="J7" s="18">
+      <c r="K7" s="18">
         <v>160</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="L7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="17">
+      <c r="M7" s="17">
         <v>1</v>
       </c>
-      <c r="M7" s="17"/>
       <c r="N7" s="17"/>
-      <c r="O7" s="17" t="s">
+      <c r="O7" s="17"/>
+      <c r="P7" s="17" t="s">
         <v>861</v>
       </c>
-      <c r="P7" s="17">
+      <c r="Q7" s="17">
         <v>1</v>
       </c>
-      <c r="Q7" s="17"/>
       <c r="R7" s="17"/>
       <c r="S7" s="17"/>
       <c r="T7" s="17"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U7" s="17"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4294,36 +4328,39 @@
       <c r="H8" s="8">
         <v>0.1</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="8">
         <v>80</v>
       </c>
-      <c r="J8" s="8">
-        <v>100</v>
-      </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="8">
+        <v>100</v>
+      </c>
+      <c r="L8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="10">
+      <c r="M8" s="10">
         <v>0.92636284614429409</v>
       </c>
-      <c r="M8" s="7" t="s">
+      <c r="N8" s="7" t="s">
         <v>830</v>
       </c>
-      <c r="N8" s="10">
+      <c r="O8" s="10">
         <v>7.3637153855705906E-2</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="P8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="P8" s="7">
+      <c r="Q8" s="7">
         <v>1</v>
       </c>
-      <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U8" s="7"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>833</v>
       </c>
@@ -4348,40 +4385,43 @@
       <c r="H9" s="8">
         <v>0.1</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="34" t="s">
+        <v>889</v>
+      </c>
+      <c r="J9" s="8">
         <v>80</v>
       </c>
-      <c r="J9" s="8">
+      <c r="K9" s="8">
         <v>70</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="L9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="10">
+      <c r="M9" s="10">
         <v>0.90716180371352784</v>
       </c>
-      <c r="M9" s="7" t="s">
+      <c r="N9" s="7" t="s">
         <v>830</v>
       </c>
-      <c r="N9" s="10">
+      <c r="O9" s="10">
         <v>9.2838196286472163E-2</v>
       </c>
-      <c r="O9" s="7" t="s">
+      <c r="P9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="10">
+      <c r="Q9" s="10">
         <v>0.30902777777777785</v>
       </c>
-      <c r="Q9" s="7" t="s">
+      <c r="R9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="R9" s="10">
+      <c r="S9" s="10">
         <v>0.6909722222222221</v>
       </c>
-      <c r="S9" s="7"/>
       <c r="T9" s="7"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U9" s="7"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>834</v>
       </c>
@@ -4406,44 +4446,47 @@
       <c r="H10" s="8">
         <v>0.1</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="34" t="s">
+        <v>889</v>
+      </c>
+      <c r="J10" s="8">
         <v>80</v>
       </c>
-      <c r="J10" s="8">
+      <c r="K10" s="8">
         <v>0</v>
       </c>
-      <c r="K10" s="7" t="s">
+      <c r="L10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L10" s="10">
+      <c r="M10" s="10">
         <v>0.90716180371352784</v>
       </c>
-      <c r="M10" s="7" t="s">
+      <c r="N10" s="7" t="s">
         <v>830</v>
       </c>
-      <c r="N10" s="10">
+      <c r="O10" s="10">
         <v>9.2838196286472163E-2</v>
       </c>
-      <c r="O10" s="7" t="s">
+      <c r="P10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="P10" s="10">
+      <c r="Q10" s="10">
         <v>0.245</v>
       </c>
-      <c r="Q10" s="7" t="s">
+      <c r="R10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="R10" s="10">
+      <c r="S10" s="10">
         <v>3.0000000000000002E-2</v>
       </c>
-      <c r="S10" s="7" t="s">
+      <c r="T10" s="7" t="s">
         <v>831</v>
       </c>
-      <c r="T10" s="10">
+      <c r="U10" s="10">
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>863</v>
       </c>
@@ -4468,38 +4511,41 @@
       <c r="H11" s="21">
         <v>0.1</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="34" t="s">
+        <v>890</v>
+      </c>
+      <c r="J11" s="21">
         <v>80</v>
       </c>
-      <c r="J11" s="21">
+      <c r="K11" s="21">
         <v>40</v>
       </c>
-      <c r="K11" s="20" t="s">
+      <c r="L11" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="20">
+      <c r="M11" s="20">
         <v>0.97731691510045371</v>
       </c>
-      <c r="M11" s="20" t="s">
+      <c r="N11" s="20" t="s">
         <v>830</v>
       </c>
-      <c r="N11" s="20">
+      <c r="O11" s="20">
         <v>2.2683084899546291E-2</v>
       </c>
-      <c r="O11" s="20" t="s">
+      <c r="P11" s="20" t="s">
         <v>861</v>
       </c>
-      <c r="P11" s="20">
+      <c r="Q11" s="20">
         <v>1</v>
       </c>
-      <c r="Q11" s="20"/>
       <c r="R11" s="20"/>
       <c r="S11" s="20"/>
       <c r="T11" s="20"/>
-      <c r="U11" s="19"/>
-      <c r="W11" s="19"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U11" s="20"/>
+      <c r="V11" s="19"/>
+      <c r="X11" s="19"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>50</v>
       </c>
@@ -4524,32 +4570,35 @@
       <c r="H12" s="8">
         <v>0</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="34" t="s">
+        <v>888</v>
+      </c>
+      <c r="J12" s="8">
         <v>240</v>
       </c>
-      <c r="J12" s="8">
+      <c r="K12" s="8">
         <v>300</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="L12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="L12" s="7">
+      <c r="M12" s="7">
         <v>1</v>
       </c>
-      <c r="M12" s="7"/>
       <c r="N12" s="7"/>
-      <c r="O12" s="7" t="s">
+      <c r="O12" s="7"/>
+      <c r="P12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="P12" s="7">
+      <c r="Q12" s="7">
         <v>1</v>
       </c>
-      <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U12" s="7"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>51</v>
       </c>
@@ -4574,32 +4623,35 @@
       <c r="H13" s="8">
         <v>0</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="34" t="s">
+        <v>888</v>
+      </c>
+      <c r="J13" s="8">
         <v>240</v>
       </c>
-      <c r="J13" s="8">
+      <c r="K13" s="8">
         <v>275</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="L13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L13" s="7">
+      <c r="M13" s="7">
         <v>1</v>
       </c>
-      <c r="M13" s="7"/>
       <c r="N13" s="7"/>
-      <c r="O13" s="7" t="s">
+      <c r="O13" s="7"/>
+      <c r="P13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="P13" s="7">
+      <c r="Q13" s="7">
         <v>1</v>
       </c>
-      <c r="Q13" s="7"/>
       <c r="R13" s="7"/>
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U13" s="7"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>44</v>
       </c>
@@ -4624,32 +4676,35 @@
       <c r="H14" s="8">
         <v>0</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="34" t="s">
+        <v>888</v>
+      </c>
+      <c r="J14" s="8">
         <v>240</v>
       </c>
-      <c r="J14" s="8">
+      <c r="K14" s="8">
         <v>225</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="L14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L14" s="7">
+      <c r="M14" s="7">
         <v>1</v>
       </c>
-      <c r="M14" s="7"/>
       <c r="N14" s="7"/>
-      <c r="O14" s="7" t="s">
+      <c r="O14" s="7"/>
+      <c r="P14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="P14" s="7">
+      <c r="Q14" s="7">
         <v>1</v>
       </c>
-      <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U14" s="7"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>45</v>
       </c>
@@ -4674,28 +4729,31 @@
       <c r="H15" s="8">
         <v>0</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="34" t="s">
+        <v>888</v>
+      </c>
+      <c r="J15" s="8">
         <v>240</v>
       </c>
-      <c r="J15" s="8">
+      <c r="K15" s="8">
         <v>175</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="L15" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L15" s="7">
+      <c r="M15" s="7">
         <v>1</v>
       </c>
-      <c r="M15" s="7"/>
       <c r="N15" s="7"/>
-      <c r="O15" s="7" t="s">
+      <c r="O15" s="7"/>
+      <c r="P15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="P15" s="7">
+      <c r="Q15" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>58</v>
       </c>
@@ -4720,28 +4778,31 @@
       <c r="H16" s="8">
         <v>0</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="34" t="s">
+        <v>888</v>
+      </c>
+      <c r="J16" s="8">
         <v>240</v>
       </c>
-      <c r="J16" s="8">
+      <c r="K16" s="8">
         <v>125</v>
       </c>
-      <c r="K16" s="7" t="s">
+      <c r="L16" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L16" s="7">
+      <c r="M16" s="7">
         <v>1</v>
       </c>
-      <c r="M16" s="7"/>
       <c r="N16" s="7"/>
-      <c r="O16" s="7" t="s">
+      <c r="O16" s="7"/>
+      <c r="P16" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="P16" s="7">
+      <c r="Q16" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>59</v>
       </c>
@@ -4766,28 +4827,31 @@
       <c r="H17" s="8">
         <v>0</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="34" t="s">
+        <v>888</v>
+      </c>
+      <c r="J17" s="8">
         <v>240</v>
       </c>
-      <c r="J17" s="8">
+      <c r="K17" s="8">
         <v>75</v>
       </c>
-      <c r="K17" s="7" t="s">
+      <c r="L17" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L17" s="7">
+      <c r="M17" s="7">
         <v>1</v>
       </c>
-      <c r="M17" s="7"/>
       <c r="N17" s="7"/>
-      <c r="O17" s="7" t="s">
+      <c r="O17" s="7"/>
+      <c r="P17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="P17" s="7">
+      <c r="Q17" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>864</v>
       </c>
@@ -4812,32 +4876,35 @@
       <c r="H18" s="34">
         <v>0</v>
       </c>
-      <c r="I18" s="34">
+      <c r="I18" s="34" t="s">
+        <v>888</v>
+      </c>
+      <c r="J18" s="34">
         <v>240</v>
       </c>
-      <c r="J18" s="23">
+      <c r="K18" s="23">
         <v>250</v>
       </c>
-      <c r="K18" s="22" t="s">
+      <c r="L18" s="22" t="s">
         <v>861</v>
       </c>
-      <c r="L18" s="22">
+      <c r="M18" s="22">
         <v>1</v>
       </c>
-      <c r="M18" s="22"/>
       <c r="N18" s="22"/>
-      <c r="O18" s="22" t="s">
+      <c r="O18" s="22"/>
+      <c r="P18" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="P18" s="22">
+      <c r="Q18" s="22">
         <v>1</v>
       </c>
-      <c r="Q18" s="22"/>
       <c r="R18" s="22"/>
       <c r="S18" s="22"/>
       <c r="T18" s="22"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U18" s="22"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
         <v>865</v>
       </c>
@@ -4862,32 +4929,35 @@
       <c r="H19" s="34">
         <v>0</v>
       </c>
-      <c r="I19" s="34">
+      <c r="I19" s="34" t="s">
+        <v>888</v>
+      </c>
+      <c r="J19" s="34">
         <v>240</v>
       </c>
-      <c r="J19" s="25">
+      <c r="K19" s="25">
         <v>200</v>
       </c>
-      <c r="K19" s="24" t="s">
+      <c r="L19" s="24" t="s">
         <v>861</v>
       </c>
-      <c r="L19" s="24">
+      <c r="M19" s="24">
         <v>1</v>
       </c>
-      <c r="M19" s="24"/>
       <c r="N19" s="24"/>
-      <c r="O19" s="24" t="s">
+      <c r="O19" s="24"/>
+      <c r="P19" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="P19" s="24">
+      <c r="Q19" s="24">
         <v>1</v>
       </c>
-      <c r="Q19" s="24"/>
       <c r="R19" s="24"/>
       <c r="S19" s="24"/>
       <c r="T19" s="24"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U19" s="24"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>866</v>
       </c>
@@ -4912,28 +4982,31 @@
       <c r="H20" s="34">
         <v>0</v>
       </c>
-      <c r="I20" s="34">
+      <c r="I20" s="34" t="s">
+        <v>888</v>
+      </c>
+      <c r="J20" s="34">
         <v>240</v>
       </c>
-      <c r="J20" s="28">
+      <c r="K20" s="28">
         <v>150</v>
       </c>
-      <c r="K20" s="27" t="s">
+      <c r="L20" s="27" t="s">
         <v>861</v>
       </c>
-      <c r="L20" s="27">
+      <c r="M20" s="27">
         <v>1</v>
       </c>
-      <c r="M20" s="27"/>
       <c r="N20" s="27"/>
-      <c r="O20" s="27" t="s">
+      <c r="O20" s="27"/>
+      <c r="P20" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="P20" s="27">
+      <c r="Q20" s="27">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>867</v>
       </c>
@@ -4958,28 +5031,31 @@
       <c r="H21" s="34">
         <v>0</v>
       </c>
-      <c r="I21" s="34">
+      <c r="I21" s="34" t="s">
+        <v>888</v>
+      </c>
+      <c r="J21" s="34">
         <v>240</v>
       </c>
-      <c r="J21" s="31">
-        <v>100</v>
-      </c>
-      <c r="K21" s="30" t="s">
+      <c r="K21" s="31">
+        <v>100</v>
+      </c>
+      <c r="L21" s="30" t="s">
         <v>861</v>
       </c>
-      <c r="L21" s="30">
+      <c r="M21" s="30">
         <v>1</v>
       </c>
-      <c r="M21" s="30"/>
       <c r="N21" s="30"/>
-      <c r="O21" s="30" t="s">
+      <c r="O21" s="30"/>
+      <c r="P21" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="P21" s="30">
+      <c r="Q21" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
         <v>868</v>
       </c>
@@ -5004,24 +5080,27 @@
       <c r="H22" s="34">
         <v>0</v>
       </c>
-      <c r="I22" s="34">
+      <c r="I22" s="34" t="s">
+        <v>888</v>
+      </c>
+      <c r="J22" s="34">
         <v>240</v>
       </c>
-      <c r="J22" s="34">
+      <c r="K22" s="34">
         <v>50</v>
       </c>
-      <c r="K22" s="33" t="s">
+      <c r="L22" s="33" t="s">
         <v>861</v>
       </c>
-      <c r="L22" s="33">
+      <c r="M22" s="33">
         <v>1</v>
       </c>
-      <c r="M22" s="33"/>
       <c r="N22" s="33"/>
-      <c r="O22" s="33" t="s">
+      <c r="O22" s="33"/>
+      <c r="P22" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="P22" s="33">
+      <c r="Q22" s="33">
         <v>1</v>
       </c>
     </row>
@@ -15317,7 +15396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>